<commit_message>
Completed applying conditional formatting to selected cells.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableWithConditionalFormatting.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableWithConditionalFormatting.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CF7A4C-CBB8-4C27-B10A-EFE68599E352}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6904D418-3198-440F-81EB-C0E2E3B01FDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" activeTab="2" xr2:uid="{8D0652A6-F9BF-490E-873C-D2B449EDD650}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" activeTab="3" xr2:uid="{8D0652A6-F9BF-490E-873C-D2B449EDD650}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="PivotTables" sheetId="24" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="29" r:id="rId3"/>
-    <sheet name="Sheet8" sheetId="27" state="veryHidden" r:id="rId4"/>
-    <sheet name="Sheet9" sheetId="28" state="veryHidden" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="30" r:id="rId4"/>
+    <sheet name="Sheet8" sheetId="27" state="veryHidden" r:id="rId5"/>
+    <sheet name="Sheet9" sheetId="28" state="veryHidden" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="103">
   <si>
     <t/>
   </si>
@@ -956,23 +957,23 @@
     <dataField name="Sum of Profit (LCY)" fld="9" baseField="0" baseItem="0"/>
   </dataFields>
   <conditionalFormats count="2">
+    <conditionalFormat priority="1">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
     <conditionalFormat scope="data" priority="2">
       <pivotAreas count="1">
         <pivotArea outline="0" fieldPosition="0">
           <references count="1">
             <reference field="4294967294" count="1" selected="0">
               <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="1">
-      <pivotAreas count="1">
-        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="1"/>
             </reference>
           </references>
         </pivotArea>
@@ -1210,7 +1211,29 @@
     <dataField name="Sum of Profit (LCY)" fld="9" baseField="0" baseItem="0"/>
   </dataFields>
   <conditionalFormats count="3">
-    <conditionalFormat scope="data" priority="1">
+    <conditionalFormat scope="data" priority="9">
+      <pivotAreas count="1">
+        <pivotArea outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat scope="data" priority="8">
+      <pivotAreas count="1">
+        <pivotArea outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat scope="data" priority="7">
       <pivotAreas count="1">
         <pivotArea outline="0" fieldPosition="0">
           <references count="1">
@@ -1221,23 +1244,463 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat scope="data" priority="2">
-      <pivotAreas count="1">
-        <pivotArea outline="0" fieldPosition="0">
-          <references count="1">
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B91FD8A2-F61F-4D44-BD45-94729C77FC25}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="B2:F17" firstHeaderRow="0" firstDataRow="1" firstDataCol="3"/>
+  <pivotFields count="10">
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="38">
+        <item x="4"/>
+        <item x="12"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="5"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="11"/>
+        <item m="1" x="21"/>
+        <item m="1" x="32"/>
+        <item m="1" x="29"/>
+        <item m="1" x="35"/>
+        <item m="1" x="20"/>
+        <item m="1" x="37"/>
+        <item m="1" x="28"/>
+        <item m="1" x="15"/>
+        <item m="1" x="25"/>
+        <item m="1" x="27"/>
+        <item m="1" x="30"/>
+        <item m="1" x="22"/>
+        <item m="1" x="18"/>
+        <item x="0"/>
+        <item m="1" x="26"/>
+        <item x="2"/>
+        <item m="1" x="34"/>
+        <item m="1" x="17"/>
+        <item m="1" x="19"/>
+        <item m="1" x="16"/>
+        <item m="1" x="33"/>
+        <item x="1"/>
+        <item m="1" x="23"/>
+        <item m="1" x="36"/>
+        <item m="1" x="14"/>
+        <item m="1" x="31"/>
+        <item m="1" x="24"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="11">
+        <item x="3"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="14" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="13">
+        <item x="10"/>
+        <item x="9"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="12"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="11"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="17">
+        <item x="4"/>
+        <item x="1"/>
+        <item m="1" x="14"/>
+        <item x="3"/>
+        <item x="7"/>
+        <item m="1" x="13"/>
+        <item m="1" x="9"/>
+        <item m="1" x="10"/>
+        <item x="2"/>
+        <item m="1" x="12"/>
+        <item m="1" x="16"/>
+        <item m="1" x="11"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item m="1" x="8"/>
+        <item x="0"/>
+        <item m="1" x="15"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="2"/>
+    <field x="4"/>
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="15">
+    <i>
+      <x/>
+      <x v="3"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="6"/>
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="4"/>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="9"/>
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="11"/>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x/>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x v="12"/>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x v="5"/>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="9"/>
+      <x/>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="10"/>
+      <x v="2"/>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Net Change" fld="7" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Outstanding Orders" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <conditionalFormats count="6">
+    <conditionalFormat priority="6">
+      <pivotAreas count="2">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
             <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="4" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="5" count="1" selected="0">
               <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="4" count="2" selected="0">
+              <x v="6"/>
+              <x v="7"/>
+            </reference>
+            <reference field="5" count="1" selected="0">
+              <x v="15"/>
             </reference>
           </references>
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat scope="data" priority="3">
+    <conditionalFormat priority="5">
       <pivotAreas count="1">
-        <pivotArea outline="0" fieldPosition="0">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="5" selected="0">
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+            </reference>
+            <reference field="4" count="4" selected="0">
+              <x v="0"/>
+              <x v="2"/>
+              <x v="5"/>
+              <x v="12"/>
+            </reference>
+            <reference field="5" count="5" selected="0">
+              <x v="4"/>
+              <x v="8"/>
+              <x v="12"/>
+              <x v="13"/>
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="4">
+      <pivotAreas count="2">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="4" count="2" selected="0">
+              <x v="7"/>
+              <x v="8"/>
+            </reference>
+            <reference field="5" count="1" selected="0">
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="8" selected="0">
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+            </reference>
+            <reference field="4" count="8" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="9"/>
+              <x v="10"/>
+              <x v="11"/>
+              <x v="12"/>
+            </reference>
+            <reference field="5" count="7" selected="0">
+              <x v="0"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="8"/>
+              <x v="12"/>
+              <x v="13"/>
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="3">
+      <pivotAreas count="2">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="4" count="1" selected="0">
+              <x v="8"/>
+            </reference>
+            <reference field="5" count="1" selected="0">
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="7" selected="0">
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+            </reference>
+            <reference field="4" count="8" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="9"/>
+              <x v="10"/>
+              <x v="11"/>
+              <x v="12"/>
+            </reference>
+            <reference field="5" count="6" selected="0">
+              <x v="0"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="8"/>
+              <x v="12"/>
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="2">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="2" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+            </reference>
+            <reference field="4" count="4" selected="0">
+              <x v="3"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+            </reference>
+            <reference field="5" count="2" selected="0">
+              <x v="1"/>
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="1">
+      <pivotAreas count="2">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="8" selected="0">
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+            </reference>
+            <reference field="4" count="8" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="5"/>
+              <x v="9"/>
+              <x v="10"/>
+              <x v="11"/>
+              <x v="12"/>
+            </reference>
+            <reference field="5" count="6" selected="0">
+              <x v="0"/>
+              <x v="4"/>
+              <x v="8"/>
+              <x v="12"/>
+              <x v="13"/>
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
             <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
+              <x v="1"/>
             </reference>
           </references>
         </pivotArea>
@@ -2626,15 +3089,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17A7DB3-405B-4481-B676-7AC4770CFBE0}">
   <dimension ref="B2:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
@@ -3026,7 +3489,7 @@
     </row>
   </sheetData>
   <conditionalFormatting pivot="1" sqref="E3:E31">
-    <cfRule type="iconSet" priority="3">
+    <cfRule type="iconSet" priority="9">
       <iconSet iconSet="5Rating">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -3037,7 +3500,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="F3:F31">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3049,7 +3512,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="G3:G31">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3085,6 +3548,368 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9263D0DA-6159-4D82-BCE6-BD526F547A35}">
+  <dimension ref="B2:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3218.1400000000003</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1">
+        <v>255797.35</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1354.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1">
+        <v>821.99999999999989</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1736.3899999999999</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4390.5199999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1">
+        <v>58518.63</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="1">
+        <v>147258.97</v>
+      </c>
+      <c r="F8" s="1">
+        <v>8548.9699999999993</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2461</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3112.13</v>
+      </c>
+      <c r="F10" s="1">
+        <v>116491.69</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1">
+        <v>86949.84</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1">
+        <v>8794.86</v>
+      </c>
+      <c r="F12" s="1">
+        <v>81399.66</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="1">
+        <v>115966.31000000001</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="1">
+        <v>537967</v>
+      </c>
+      <c r="F14" s="1">
+        <v>10820.18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="1">
+        <v>7841.0000000000009</v>
+      </c>
+      <c r="F15" s="1">
+        <v>6272.81</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="1">
+        <v>200615.42</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1431059.04</v>
+      </c>
+      <c r="F17" s="1">
+        <v>229278.33</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting pivot="1" sqref="E4:E5 E3">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="E12:E16">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="E5:E6 E7:E15">
+    <cfRule type="iconSet" priority="4">
+      <iconSet iconSet="3Flags">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="F7:F14 F6">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{21CF17A0-A6AE-4149-B08C-1DEFE154AC6E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="F3:F6">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF7030A0"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="F8:F16 F17">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" pivot="1">
+          <x14:cfRule type="dataBar" id="{21CF17A0-A6AE-4149-B08C-1DEFE154AC6E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F7:F14 F6</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B2DE5A-B0CE-40B0-B90A-13DD0645D08A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -3130,7 +3955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CC8136-0242-4B7D-9D2E-D523319B4548}">
   <dimension ref="A1:D9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Minor fix in updating pivot table conditional formatting references and added more tests.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableWithConditionalFormatting.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableWithConditionalFormatting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6904D418-3198-440F-81EB-C0E2E3B01FDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3084EE-B68A-4181-8C3C-E2D8FA2C6CAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" activeTab="3" xr2:uid="{8D0652A6-F9BF-490E-873C-D2B449EDD650}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="2" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="118">
   <si>
     <t/>
   </si>
@@ -347,6 +347,51 @@
   </si>
   <si>
     <t>Sum of Outstanding Orders</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Antarcticopy Total</t>
+  </si>
+  <si>
+    <t>Autohaus Mielberg KG Total</t>
+  </si>
+  <si>
+    <t>BYT-KOMPLET s.r.o. Total</t>
+  </si>
+  <si>
+    <t>Deerfield Graphics Company Total</t>
+  </si>
+  <si>
+    <t>Designstudio Gmunden Total</t>
+  </si>
+  <si>
+    <t>Englunds Kontorsmöbler AB Total</t>
+  </si>
+  <si>
+    <t>Gagn &amp; Gaman Total</t>
+  </si>
+  <si>
+    <t>Guildford Water Department Total</t>
+  </si>
+  <si>
+    <t>Heimilisprydi Total</t>
+  </si>
+  <si>
+    <t>John Haddock Insurance Co. Total</t>
+  </si>
+  <si>
+    <t>Klubben Total</t>
+  </si>
+  <si>
+    <t>Progressive Home Furnishings Total</t>
+  </si>
+  <si>
+    <t>Selangorian Ltd. Total</t>
+  </si>
+  <si>
+    <t>The Cannon Group PLC Total</t>
   </si>
 </sst>
 </file>
@@ -382,13 +427,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,7 +810,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E03B6EC8-4332-451F-A0F6-B96CBB15FE94}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E03B6EC8-4332-451F-A0F6-B96CBB15FE94}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="B2:F17" firstHeaderRow="0" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="10">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
@@ -957,23 +1011,23 @@
     <dataField name="Sum of Profit (LCY)" fld="9" baseField="0" baseItem="0"/>
   </dataFields>
   <conditionalFormats count="2">
+    <conditionalFormat scope="data" priority="2">
+      <pivotAreas count="1">
+        <pivotArea outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
     <conditionalFormat priority="1">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="1">
             <reference field="4294967294" count="1" selected="0">
               <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat scope="data" priority="2">
-      <pivotAreas count="1">
-        <pivotArea outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
             </reference>
           </references>
         </pivotArea>
@@ -993,7 +1047,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96563FC8-2A56-451F-9412-65E8E6860C30}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96563FC8-2A56-451F-9412-65E8E6860C30}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="B2:G31" firstHeaderRow="0" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="10">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
@@ -1211,12 +1265,12 @@
     <dataField name="Sum of Profit (LCY)" fld="9" baseField="0" baseItem="0"/>
   </dataFields>
   <conditionalFormats count="3">
-    <conditionalFormat scope="data" priority="9">
+    <conditionalFormat scope="data" priority="7">
       <pivotAreas count="1">
         <pivotArea outline="0" fieldPosition="0">
           <references count="1">
             <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
+              <x v="2"/>
             </reference>
           </references>
         </pivotArea>
@@ -1233,12 +1287,12 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat scope="data" priority="7">
+    <conditionalFormat scope="data" priority="9">
       <pivotAreas count="1">
         <pivotArea outline="0" fieldPosition="0">
           <references count="1">
             <reference field="4294967294" count="1" selected="0">
-              <x v="2"/>
+              <x v="0"/>
             </reference>
           </references>
         </pivotArea>
@@ -1258,7 +1312,928 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B91FD8A2-F61F-4D44-BD45-94729C77FC25}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{565AB755-91E1-4294-BEEF-F647FABB0596}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I2:K39" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="12">
+        <item x="3"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="14">
+        <item x="10"/>
+        <item x="9"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="12"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="18">
+        <item x="4"/>
+        <item x="1"/>
+        <item m="1" x="14"/>
+        <item x="3"/>
+        <item x="7"/>
+        <item m="1" x="13"/>
+        <item m="1" x="9"/>
+        <item m="1" x="10"/>
+        <item x="2"/>
+        <item m="1" x="12"/>
+        <item m="1" x="16"/>
+        <item m="1" x="11"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item m="1" x="8"/>
+        <item x="0"/>
+        <item m="1" x="15"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="2"/>
+    <field x="5"/>
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="37">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="2">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="7"/>
+    </i>
+    <i r="2">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Net Change" fld="7" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Outstanding Orders" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <conditionalFormats count="3">
+    <conditionalFormat scope="field" priority="3">
+      <pivotAreas count="1">
+        <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="0" selected="0"/>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="2">
+      <pivotAreas count="12">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="5" count="1">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="4" count="1">
+              <x v="3"/>
+            </reference>
+            <reference field="5" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="5" count="1">
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="4" count="3">
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+            </reference>
+            <reference field="5" count="1" selected="0">
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1">
+              <x v="2"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="5" count="1">
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="4" count="1">
+              <x v="4"/>
+            </reference>
+            <reference field="5" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1">
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="5" count="1">
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="4" count="2">
+              <x v="9"/>
+              <x v="10"/>
+            </reference>
+            <reference field="5" count="1" selected="0">
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="1">
+      <pivotAreas count="15">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1">
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="5" count="1">
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="4" count="2">
+              <x v="9"/>
+              <x v="10"/>
+            </reference>
+            <reference field="5" count="1" selected="0">
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1">
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="5" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="4" count="1">
+              <x v="1"/>
+            </reference>
+            <reference field="5" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1">
+              <x v="5"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="5"/>
+            </reference>
+            <reference field="5" count="1">
+              <x v="8"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="5"/>
+            </reference>
+            <reference field="4" count="1">
+              <x v="11"/>
+            </reference>
+            <reference field="5" count="1" selected="0">
+              <x v="8"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1">
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="6"/>
+            </reference>
+            <reference field="5" count="1">
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="6"/>
+            </reference>
+            <reference field="4" count="1">
+              <x v="0"/>
+            </reference>
+            <reference field="5" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1">
+              <x v="7"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="7"/>
+            </reference>
+            <reference field="5" count="1">
+              <x v="12"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="4">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="7"/>
+            </reference>
+            <reference field="4" count="1">
+              <x v="12"/>
+            </reference>
+            <reference field="5" count="1" selected="0">
+              <x v="12"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6CA5165F-07ED-41DE-90E0-72D538DF66A4}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B23:F66" firstHeaderRow="0" firstDataRow="1" firstDataCol="3"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" outline="0" showAll="0">
+      <items count="39">
+        <item x="4"/>
+        <item x="12"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="5"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="11"/>
+        <item m="1" x="21"/>
+        <item m="1" x="32"/>
+        <item m="1" x="29"/>
+        <item m="1" x="35"/>
+        <item m="1" x="20"/>
+        <item m="1" x="37"/>
+        <item m="1" x="28"/>
+        <item m="1" x="15"/>
+        <item m="1" x="25"/>
+        <item m="1" x="27"/>
+        <item m="1" x="30"/>
+        <item m="1" x="22"/>
+        <item m="1" x="18"/>
+        <item x="0"/>
+        <item m="1" x="26"/>
+        <item x="2"/>
+        <item m="1" x="34"/>
+        <item m="1" x="17"/>
+        <item m="1" x="19"/>
+        <item m="1" x="16"/>
+        <item m="1" x="33"/>
+        <item x="1"/>
+        <item m="1" x="23"/>
+        <item m="1" x="36"/>
+        <item m="1" x="14"/>
+        <item m="1" x="31"/>
+        <item m="1" x="24"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" showAll="0">
+      <items count="12">
+        <item x="3"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="14">
+        <item x="10"/>
+        <item x="9"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="12"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="18">
+        <item x="4"/>
+        <item x="1"/>
+        <item m="1" x="14"/>
+        <item x="3"/>
+        <item x="7"/>
+        <item m="1" x="13"/>
+        <item m="1" x="9"/>
+        <item m="1" x="10"/>
+        <item x="2"/>
+        <item m="1" x="12"/>
+        <item m="1" x="16"/>
+        <item m="1" x="11"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item m="1" x="8"/>
+        <item x="0"/>
+        <item m="1" x="15"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="1"/>
+    <field x="2"/>
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="43">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="15"/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i t="default">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="8"/>
+    </i>
+    <i t="default">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="15"/>
+    </i>
+    <i t="default">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="8"/>
+    </i>
+    <i t="default">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+      <x v="8"/>
+    </i>
+    <i r="2">
+      <x v="15"/>
+    </i>
+    <i t="default">
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+      <x v="7"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i t="default">
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="24"/>
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="15"/>
+    </i>
+    <i t="default">
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="26"/>
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="15"/>
+    </i>
+    <i t="default">
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="32"/>
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="15"/>
+    </i>
+    <i t="default">
+      <x v="32"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Net Change" fld="7" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Outstanding Orders" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <conditionalFormats count="2">
+    <conditionalFormat scope="field" priority="6">
+      <pivotAreas count="1">
+        <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="0" selected="0"/>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat scope="field" priority="4">
+      <pivotAreas count="1">
+        <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="0" selected="0"/>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B91FD8A2-F61F-4D44-BD45-94729C77FC25}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="B2:F17" firstHeaderRow="0" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="10">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
@@ -1456,7 +2431,7 @@
     <dataField name="Sum of Outstanding Orders" fld="8" baseField="0" baseItem="0"/>
   </dataFields>
   <conditionalFormats count="6">
-    <conditionalFormat priority="6">
+    <conditionalFormat priority="12">
       <pivotAreas count="2">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="4">
@@ -1493,7 +2468,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="5">
+    <conditionalFormat priority="11">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="4">
@@ -1524,7 +2499,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="4">
+    <conditionalFormat priority="10">
       <pivotAreas count="2">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="4">
@@ -1581,7 +2556,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="3">
+    <conditionalFormat priority="9">
       <pivotAreas count="2">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="4">
@@ -1635,7 +2610,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="2">
+    <conditionalFormat priority="8">
       <pivotAreas count="1">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="4">
@@ -1660,7 +2635,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="1">
+    <conditionalFormat priority="7">
       <pivotAreas count="2">
         <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="4">
@@ -3549,22 +4524,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9263D0DA-6159-4D82-BCE6-BD526F547A35}">
-  <dimension ref="B2:F17"/>
+  <dimension ref="B2:K66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
@@ -3580,8 +4558,17 @@
       <c r="F2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -3597,8 +4584,17 @@
       <c r="F3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>3218.1400000000003</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>47</v>
       </c>
@@ -3614,8 +4610,17 @@
       <c r="F4" s="1">
         <v>1354.5</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>3218.1400000000003</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>93</v>
       </c>
@@ -3628,8 +4633,17 @@
       <c r="F5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1">
+        <v>3218.1400000000003</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>72</v>
       </c>
@@ -3642,8 +4656,17 @@
       <c r="F6" s="1">
         <v>4390.5199999999995</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="1">
+        <v>258355.74000000002</v>
+      </c>
+      <c r="K6" s="1">
+        <v>5745.0199999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>36</v>
       </c>
@@ -3659,8 +4682,17 @@
       <c r="F7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="1">
+        <v>258355.74000000002</v>
+      </c>
+      <c r="K7" s="1">
+        <v>5745.0199999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>44</v>
       </c>
@@ -3676,8 +4708,17 @@
       <c r="F8" s="1">
         <v>8548.9699999999993</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="1">
+        <v>255797.35</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1354.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>45</v>
       </c>
@@ -3690,8 +4731,17 @@
       <c r="F9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I9" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9" s="1">
+        <v>821.99999999999989</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>76</v>
       </c>
@@ -3707,8 +4757,17 @@
       <c r="F10" s="1">
         <v>116491.69</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I10" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1736.3899999999999</v>
+      </c>
+      <c r="K10" s="1">
+        <v>4390.5199999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>62</v>
       </c>
@@ -3724,8 +4783,17 @@
       <c r="F11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="1">
+        <v>58518.63</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>5</v>
       </c>
@@ -3741,8 +4809,17 @@
       <c r="F12" s="1">
         <v>81399.66</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="1">
+        <v>58518.63</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>88</v>
       </c>
@@ -3758,8 +4835,17 @@
       <c r="F13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="1">
+        <v>58518.63</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>41</v>
       </c>
@@ -3775,8 +4861,17 @@
       <c r="F14" s="1">
         <v>10820.18</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14" s="1">
+        <v>149719.97</v>
+      </c>
+      <c r="K14" s="1">
+        <v>8548.9699999999993</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>83</v>
       </c>
@@ -3792,8 +4887,17 @@
       <c r="F15" s="1">
         <v>6272.81</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="1">
+        <v>149719.97</v>
+      </c>
+      <c r="K15" s="1">
+        <v>8548.9699999999993</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>67</v>
       </c>
@@ -3809,8 +4913,17 @@
       <c r="F16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="I16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" s="1">
+        <v>147258.97</v>
+      </c>
+      <c r="K16" s="1">
+        <v>8548.9699999999993</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>95</v>
       </c>
@@ -3820,10 +4933,755 @@
       <c r="F17" s="1">
         <v>229278.33</v>
       </c>
+      <c r="I17" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="1">
+        <v>2461</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I18" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" s="1">
+        <v>3112.13</v>
+      </c>
+      <c r="K18" s="1">
+        <v>116491.69</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I19" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" s="1">
+        <v>3112.13</v>
+      </c>
+      <c r="K19" s="1">
+        <v>116491.69</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I20" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J20" s="1">
+        <v>3112.13</v>
+      </c>
+      <c r="K20" s="1">
+        <v>116491.69</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J21" s="1">
+        <v>86949.84</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I22" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" s="1">
+        <v>86949.84</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" t="s">
+        <v>102</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" s="1">
+        <v>86949.84</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3218.1400000000003</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J24" s="1">
+        <v>8794.86</v>
+      </c>
+      <c r="K24" s="1">
+        <v>81399.66</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D25" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3218.1400000000003</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" s="1">
+        <v>8794.86</v>
+      </c>
+      <c r="K25" s="1">
+        <v>81399.66</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="1">
+        <v>3218.1400000000003</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="8"/>
+      <c r="J26" s="1">
+        <v>8794.86</v>
+      </c>
+      <c r="K26" s="1">
+        <v>81399.66</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="1">
+        <v>8794.86</v>
+      </c>
+      <c r="F27" s="1">
+        <v>81399.66</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J27" s="1">
+        <v>115966.31000000001</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="1">
+        <v>8794.86</v>
+      </c>
+      <c r="F28" s="1">
+        <v>81399.66</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J28" s="1">
+        <v>115966.31000000001</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="1">
+        <v>8794.86</v>
+      </c>
+      <c r="F29" s="1">
+        <v>81399.66</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J29" s="1">
+        <v>115966.31000000001</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" s="1">
+        <v>58518.63</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J30" s="1">
+        <v>537967</v>
+      </c>
+      <c r="K30" s="1">
+        <v>10820.18</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="1">
+        <v>58518.63</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" s="1">
+        <v>537967</v>
+      </c>
+      <c r="K31" s="1">
+        <v>10820.18</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="1">
+        <v>58518.63</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J32" s="1">
+        <v>537967</v>
+      </c>
+      <c r="K32" s="1">
+        <v>10820.18</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B33" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1736.3899999999999</v>
+      </c>
+      <c r="F33" s="1">
+        <v>4390.5199999999995</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J33" s="1">
+        <v>7841.0000000000009</v>
+      </c>
+      <c r="K33" s="1">
+        <v>6272.81</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D34" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1736.3899999999999</v>
+      </c>
+      <c r="F34" s="1">
+        <v>4390.5199999999995</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J34" s="1">
+        <v>7841.0000000000009</v>
+      </c>
+      <c r="K34" s="1">
+        <v>6272.81</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B35" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1736.3899999999999</v>
+      </c>
+      <c r="F35" s="1">
+        <v>4390.5199999999995</v>
+      </c>
+      <c r="I35" s="8"/>
+      <c r="J35" s="1">
+        <v>7841.0000000000009</v>
+      </c>
+      <c r="K35" s="1">
+        <v>6272.81</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B36" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="1">
+        <v>3112.13</v>
+      </c>
+      <c r="F36" s="1">
+        <v>116491.69</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J36" s="1">
+        <v>200615.42</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D37" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="1">
+        <v>3112.13</v>
+      </c>
+      <c r="F37" s="1">
+        <v>116491.69</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J37" s="1">
+        <v>200615.42</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B38" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E38" s="1">
+        <v>3112.13</v>
+      </c>
+      <c r="F38" s="1">
+        <v>116491.69</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J38" s="1">
+        <v>200615.42</v>
+      </c>
+      <c r="K38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B39" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="1">
+        <v>7841.0000000000009</v>
+      </c>
+      <c r="F39" s="1">
+        <v>6272.81</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="J39" s="1">
+        <v>1431059.04</v>
+      </c>
+      <c r="K39" s="1">
+        <v>229278.33</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D40" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" s="1">
+        <v>7841.0000000000009</v>
+      </c>
+      <c r="F40" s="1">
+        <v>6272.81</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B41" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E41" s="1">
+        <v>7841.0000000000009</v>
+      </c>
+      <c r="F41" s="1">
+        <v>6272.81</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B42" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="1">
+        <v>86949.84</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D43" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E43" s="1">
+        <v>86949.84</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B44" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E44" s="1">
+        <v>86949.84</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B45" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E45" s="1">
+        <v>821.99999999999989</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D46" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" s="1">
+        <v>821.99999999999989</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B47" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E47" s="1">
+        <v>821.99999999999989</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B48" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" s="1">
+        <v>200615.42</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D49" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49" s="1">
+        <v>200615.42</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B50" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E50" s="1">
+        <v>200615.42</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E51" s="1">
+        <v>537967</v>
+      </c>
+      <c r="F51" s="1">
+        <v>10820.18</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D52" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" s="1">
+        <v>537967</v>
+      </c>
+      <c r="F52" s="1">
+        <v>10820.18</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E53" s="1">
+        <v>537967</v>
+      </c>
+      <c r="F53" s="1">
+        <v>10820.18</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E54" s="1">
+        <v>115966.31000000001</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D55" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E55" s="1">
+        <v>115966.31000000001</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B56" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E56" s="1">
+        <v>115966.31000000001</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B57" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E57" s="1">
+        <v>2461</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D58" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" s="1">
+        <v>2461</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B59" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E59" s="1">
+        <v>2461</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B60" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E60" s="1">
+        <v>147258.97</v>
+      </c>
+      <c r="F60" s="1">
+        <v>8548.9699999999993</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D61" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E61" s="1">
+        <v>147258.97</v>
+      </c>
+      <c r="F61" s="1">
+        <v>8548.9699999999993</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B62" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E62" s="1">
+        <v>147258.97</v>
+      </c>
+      <c r="F62" s="1">
+        <v>8548.9699999999993</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B63" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E63" s="1">
+        <v>255797.35</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1354.5</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D64" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64" s="1">
+        <v>255797.35</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1354.5</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B65" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E65" s="1">
+        <v>255797.35</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1354.5</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B66" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E66" s="1">
+        <v>1431059.0400000003</v>
+      </c>
+      <c r="F66" s="1">
+        <v>229278.33</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting pivot="1" sqref="E4:E5 E3">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3833,7 +5691,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="E12:E16">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3845,7 +5703,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="E5:E6 E7:E15">
-    <cfRule type="iconSet" priority="4">
+    <cfRule type="iconSet" priority="10">
       <iconSet iconSet="3Flags">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -3854,7 +5712,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="F7:F14 F6">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3868,7 +5726,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="F3:F6">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3878,8 +5736,69 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="F8:F16 F17">
+    <cfRule type="iconSet" priority="7">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="E26 E29 E32 E35 E38 E41 E44 E47 E50 E53 E56 E59 E62 E65">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="F27 F24 F30 F33 F36 F39 F42 F45 F48 F51 F54 F57 F60 F63">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{DFB22B56-2E33-4B9E-AB6C-D5BF9B57B846}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="J6 J3 J11 J14 J18 J21 J24 J27 J30 J33 J36">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="K3 K4 K5 K6 K7 K8:K10 K11 K12 K13 K14 K15 K16:K17">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E60E93BF-E954-4074-8141-F9531DAB1DD4}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="K14 K15 K16:K17 K18 K19 K20 K21 K22 K23 K24 K25 K26 K27 K28 K29">
     <cfRule type="iconSet" priority="1">
-      <iconSet iconSet="3Arrows">
+      <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
         <cfvo type="percent" val="67"/>
@@ -3903,6 +5822,28 @@
           </x14:cfRule>
           <xm:sqref>F7:F14 F6</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" pivot="1">
+          <x14:cfRule type="dataBar" id="{DFB22B56-2E33-4B9E-AB6C-D5BF9B57B846}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F27 F24 F30 F33 F36 F39 F42 F45 F48 F51 F54 F57 F60 F63</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" pivot="1">
+          <x14:cfRule type="dataBar" id="{E60E93BF-E954-4074-8141-F9531DAB1DD4}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K3 K4 K5 K6 K7 K8:K10 K11 K12 K13 K14 K15 K16:K17</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>